<commit_message>
JSTL Function Tags - split and join
</commit_message>
<xml_diff>
--- a/me_docs/6.JSP-Standard-Tag-Library-Function-Tags.xlsx
+++ b/me_docs/6.JSP-Standard-Tag-Library-Function-Tags.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\JSP-Servlets-JDBC\me_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B929385-169C-4457-A2B9-79B317810D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A15B8FE8-D341-4F43-8FE9-0DE5F6BC0710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tag" sheetId="1" r:id="rId1"/>
-    <sheet name="length-toUpperCase-startsWith" sheetId="2" r:id="rId2"/>
+    <sheet name="function-test" sheetId="2" r:id="rId2"/>
+    <sheet name="split-join-test" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,12 +27,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Create function-test.jsp</t>
   </si>
   <si>
     <t>Access URL to test: http://localhost:8080/tagdemo/function-test.jsp</t>
+  </si>
+  <si>
+    <t>Create split-join-test.jsp</t>
+  </si>
+  <si>
+    <t>Access URL to test: http://localhost:8080/tagdemo/split-join-test.jsp</t>
   </si>
 </sst>
 </file>
@@ -311,6 +318,187 @@
         <a:xfrm>
           <a:off x="609600" y="16764000"/>
           <a:ext cx="4200000" cy="1742857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>141790</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>170857</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{150170EE-7D88-4EC1-B334-49182FE70976}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="381000"/>
+          <a:ext cx="8676190" cy="4742857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>608990</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>151690</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E428AB3E-695A-40D8-982B-5E47E80788C3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="5334000"/>
+          <a:ext cx="4876190" cy="5676190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>237105</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>151762</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25BC8B4F-8311-4751-B82E-FDEFCF4C098E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="11239500"/>
+          <a:ext cx="8161905" cy="5104762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304305</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>180643</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05417311-F0E1-4E54-8766-405CBE300D21}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="16764000"/>
+          <a:ext cx="3961905" cy="2657143"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -602,8 +790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBB494D2-8A67-4E7F-88F1-14ADB29188B3}">
   <dimension ref="A2:A88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="B98" sqref="B98"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,4 +810,30 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B195A9EF-7671-4C3D-94EB-EA4E650C9126}">
+  <dimension ref="A2:A88"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="N103" sqref="N103"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>